<commit_message>
Revert "Merge branch 'master' of https://github.com/zmcgrath96/Doodle"
This reverts commit 79a3f99cd4cb6e04858a44dec8c8e45ba0d1246a, reversing
changes made to ccffba08bb061fbb38dba1583120c204a3c585ff.
</commit_message>
<xml_diff>
--- a/documentation/Meeting Log.xlsx
+++ b/documentation/Meeting Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\GitHub\Doodle\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Doodle\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Day</t>
   </si>
@@ -96,24 +96,6 @@
   </si>
   <si>
     <t>Finalize new classes and start fixing bugs</t>
-  </si>
-  <si>
-    <t>3-5 pm</t>
-  </si>
-  <si>
-    <t>Eaton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Got the sln file to finally work and </t>
-  </si>
-  <si>
-    <t>made changes to Event and Task</t>
-  </si>
-  <si>
-    <t>Read/Write, Other stuff</t>
-  </si>
-  <si>
-    <t>Kind of?</t>
   </si>
 </sst>
 </file>
@@ -142,7 +124,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,12 +161,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -198,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,12 +204,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -526,7 +496,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,34 +642,20 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
-        <v>43157</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/zmcgrath96/Doodle""
This reverts commit 1435ab9964c7e628fd399f292bdb9476eba37f89.
</commit_message>
<xml_diff>
--- a/documentation/Meeting Log.xlsx
+++ b/documentation/Meeting Log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Doodle\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach\Documents\GitHub\Doodle\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Day</t>
   </si>
@@ -96,6 +96,24 @@
   </si>
   <si>
     <t>Finalize new classes and start fixing bugs</t>
+  </si>
+  <si>
+    <t>3-5 pm</t>
+  </si>
+  <si>
+    <t>Eaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Got the sln file to finally work and </t>
+  </si>
+  <si>
+    <t>made changes to Event and Task</t>
+  </si>
+  <si>
+    <t>Read/Write, Other stuff</t>
+  </si>
+  <si>
+    <t>Kind of?</t>
   </si>
 </sst>
 </file>
@@ -124,7 +142,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +179,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -174,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,6 +228,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -496,7 +526,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,20 +672,34 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="11">
+        <v>43157</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>

</xml_diff>